<commit_message>
Env Settings for Attachment Path
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://learnermanipal-my.sharepoint.com/personal/rishabh_jain1_learner_manipal_edu/Documents/Coding/Mini-Projects/Auto-Mailer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\OneDrive - Manipal Academy of Higher Education\Coding\Mini-Projects\Auto-Mailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{0DCBC7F7-EC0D-4710-BA1F-977DEF828F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D543715-7C11-4F25-842E-783090C4E7CC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615D8414-7743-41F4-8B23-06A01A43A0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -379,7 +379,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>